<commit_message>
Update Playground - Conditional Formatting.xlsx
</commit_message>
<xml_diff>
--- a/Playground - Conditional Formatting.xlsx
+++ b/Playground - Conditional Formatting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3713F0A-9C9D-4283-AE83-BC349FBC7021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199C39D7-D5CC-439C-87CB-A6273DF1C91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027015F-D30F-450C-928C-DE78480974B7}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3CCAA7F-6F85-4102-B7D4-D80770622F9F}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>